<commit_message>
+ add sandler's program.
</commit_message>
<xml_diff>
--- a/dcec/adddomain/yyedaddpm/cim.xlsx
+++ b/dcec/adddomain/yyedaddpm/cim.xlsx
@@ -28,6 +28,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>必须要以</t>
@@ -48,6 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">开头
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>gplblmt.p</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -263,6 +265,10 @@
   </si>
   <si>
     <t>传输命令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BACKUP_FILES_DIR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -274,7 +280,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,11 +291,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -304,7 +312,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -341,7 +358,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -349,6 +366,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -650,7 +670,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.5"/>
@@ -773,8 +793,8 @@
       <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
-        <v>53</v>
+      <c r="B7" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>

</xml_diff>